<commit_message>
Add Authentication test cases
</commit_message>
<xml_diff>
--- a/report/sheet_wise_Tc.xlsx
+++ b/report/sheet_wise_Tc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ai-quizwhiz.zluck.com-pnt-b24\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\my github project\ai-quizwhiz.zluck.com-pnt-b24\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -985,7 +985,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M18" sqref="M18"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>